<commit_message>
Nos queremos pegar un tirito
</commit_message>
<xml_diff>
--- a/Cirel/Practica 4/CIREL.xlsx
+++ b/Cirel/Practica 4/CIREL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>Frecuencia(Hz)</t>
   </si>
@@ -276,6 +276,75 @@
   <si>
     <t>V2(V)</t>
   </si>
+  <si>
+    <t>4,2ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,9ms </t>
+  </si>
+  <si>
+    <t>2,2ms</t>
+  </si>
+  <si>
+    <t>1,9ms</t>
+  </si>
+  <si>
+    <t>720μs</t>
+  </si>
+  <si>
+    <t>360μs</t>
+  </si>
+  <si>
+    <t>200μs</t>
+  </si>
+  <si>
+    <t>140μs</t>
+  </si>
+  <si>
+    <t>90μs</t>
+  </si>
+  <si>
+    <t>60μs</t>
+  </si>
+  <si>
+    <t>44μs</t>
+  </si>
+  <si>
+    <t>40μs</t>
+  </si>
+  <si>
+    <t>7μs</t>
+  </si>
+  <si>
+    <t>2,8μs</t>
+  </si>
+  <si>
+    <t>1,6μs</t>
+  </si>
+  <si>
+    <t>1μs</t>
+  </si>
+  <si>
+    <t>700ns</t>
+  </si>
+  <si>
+    <t>500ns</t>
+  </si>
+  <si>
+    <t>300ns</t>
+  </si>
+  <si>
+    <t>100ns</t>
+  </si>
+  <si>
+    <t>80ns</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>40ns</t>
+  </si>
 </sst>
 </file>
 
@@ -283,7 +352,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.0000\ _€_-;\-* #,##0.0000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0000\ _€_-;\-* #,##0.0000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -333,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -623,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M30"/>
+  <dimension ref="B1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +707,7 @@
     <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>30</v>
       </c>
@@ -654,7 +723,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>50</v>
       </c>
@@ -706,17 +775,29 @@
       <c r="I4" s="1">
         <v>50</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1">
+        <f>N4/2</f>
+        <v>0.59</v>
+      </c>
       <c r="K4" s="1">
         <v>2.04</v>
       </c>
       <c r="L4" s="2">
         <f>J4/K4</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+        <v>0.28921568627450978</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4">
+        <f>O4*10</f>
+        <v>1.18</v>
+      </c>
+      <c r="O4">
+        <v>0.11799999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>70</v>
       </c>
@@ -736,17 +817,29 @@
       <c r="I5" s="1">
         <v>70</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1">
+        <f t="shared" ref="J5:J30" si="1">N5/2</f>
+        <v>0.79</v>
+      </c>
       <c r="K5" s="1">
         <v>2.04</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" ref="L5:L30" si="1">J5/K5</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" ref="L5:L30" si="2">J5/K5</f>
+        <v>0.38725490196078433</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N30" si="3">O5*10</f>
+        <v>1.58</v>
+      </c>
+      <c r="O5">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>90</v>
       </c>
@@ -766,17 +859,29 @@
       <c r="I6" s="1">
         <v>90</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.97</v>
+      </c>
       <c r="K6" s="1">
         <v>2.04</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.47549019607843135</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>1.94</v>
+      </c>
+      <c r="O6">
+        <v>0.19400000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>100</v>
       </c>
@@ -796,17 +901,29 @@
       <c r="I7" s="1">
         <v>100</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>1.05</v>
+      </c>
       <c r="K7" s="1">
         <v>2.04</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.51470588235294124</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+      <c r="O7">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>200</v>
       </c>
@@ -826,17 +943,29 @@
       <c r="I8" s="1">
         <v>200</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.55</v>
+      </c>
       <c r="K8" s="1">
         <v>2.04</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.75980392156862742</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>3.1</v>
+      </c>
+      <c r="O8">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>300</v>
       </c>
@@ -856,17 +985,29 @@
       <c r="I9" s="1">
         <v>300</v>
       </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7799999999999998</v>
+      </c>
       <c r="K9" s="1">
         <v>2.04</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.87254901960784303</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>3.5599999999999996</v>
+      </c>
+      <c r="O9">
+        <v>0.35599999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>400</v>
       </c>
@@ -886,17 +1027,29 @@
       <c r="I10" s="1">
         <v>400</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8599999999999999</v>
+      </c>
       <c r="K10" s="1">
         <v>2.04</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.91176470588235281</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>3.7199999999999998</v>
+      </c>
+      <c r="O10">
+        <v>0.372</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>500</v>
       </c>
@@ -916,17 +1069,29 @@
       <c r="I11" s="1">
         <v>500</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.87</v>
+      </c>
       <c r="K11" s="1">
         <v>2.04</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.91666666666666674</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>3.74</v>
+      </c>
+      <c r="O11">
+        <v>0.374</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>600</v>
       </c>
@@ -946,17 +1111,29 @@
       <c r="I12" s="1">
         <v>600</v>
       </c>
-      <c r="J12" s="1"/>
+      <c r="J12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.92</v>
+      </c>
       <c r="K12" s="1">
         <v>2.04</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>3.84</v>
+      </c>
+      <c r="O12">
+        <v>0.38400000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>700</v>
       </c>
@@ -976,17 +1153,29 @@
       <c r="I13" s="1">
         <v>700</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K13" s="1">
         <v>2.04</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O13">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>800</v>
       </c>
@@ -1006,17 +1195,29 @@
       <c r="I14" s="1">
         <v>800</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K14" s="1">
         <v>2.04</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O14">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>900</v>
       </c>
@@ -1036,17 +1237,29 @@
       <c r="I15" s="1">
         <v>900</v>
       </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K15" s="1">
         <v>2.04</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O15">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>1000</v>
       </c>
@@ -1066,17 +1279,29 @@
       <c r="I16" s="1">
         <v>1000</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K16" s="1">
         <v>2.04</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O16">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>2000</v>
       </c>
@@ -1096,17 +1321,29 @@
       <c r="I17" s="1">
         <v>2000</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K17" s="1">
         <v>2.04</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O17">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>3000</v>
       </c>
@@ -1126,17 +1363,29 @@
       <c r="I18" s="1">
         <v>3000</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K18" s="1">
         <v>2.04</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O18">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>3500</v>
       </c>
@@ -1156,17 +1405,29 @@
       <c r="I19" s="1">
         <v>3500</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K19" s="1">
         <v>2.04</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O19">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>4000</v>
       </c>
@@ -1186,17 +1447,29 @@
       <c r="I20" s="1">
         <v>4000</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K20" s="1">
         <v>2.04</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O20">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>4500</v>
       </c>
@@ -1216,17 +1489,29 @@
       <c r="I21" s="1">
         <v>4500</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K21" s="1">
         <v>2.04</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M21" s="3"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O21">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>5000</v>
       </c>
@@ -1246,17 +1531,29 @@
       <c r="I22" s="1">
         <v>5000</v>
       </c>
-      <c r="J22" s="1"/>
+      <c r="J22" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K22" s="1">
         <v>2.04</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O22">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>6000</v>
       </c>
@@ -1276,17 +1573,29 @@
       <c r="I23" s="1">
         <v>6000</v>
       </c>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K23" s="1">
         <v>2.04</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O23">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>7000</v>
       </c>
@@ -1306,17 +1615,29 @@
       <c r="I24" s="1">
         <v>7000</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K24" s="1">
         <v>2.04</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="3"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O24">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>8000</v>
       </c>
@@ -1336,17 +1657,29 @@
       <c r="I25" s="1">
         <v>8000</v>
       </c>
-      <c r="J25" s="1"/>
+      <c r="J25" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K25" s="1">
         <v>2.04</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O25">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>9000</v>
       </c>
@@ -1366,17 +1699,29 @@
       <c r="I26" s="1">
         <v>9000</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="J26" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K26" s="1">
         <v>2.04</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M26" s="3"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O26">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>10000</v>
       </c>
@@ -1396,17 +1741,29 @@
       <c r="I27" s="1">
         <v>10000</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K27" s="1">
         <v>2.04</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O27">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>20000</v>
       </c>
@@ -1426,17 +1783,29 @@
       <c r="I28" s="1">
         <v>20000</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K28" s="1">
         <v>2.04</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M28" s="1"/>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O28">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>30000</v>
       </c>
@@ -1456,17 +1825,29 @@
       <c r="I29" s="1">
         <v>30000</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="J29" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K29" s="1">
         <v>2.04</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O29">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>50000</v>
       </c>
@@ -1486,15 +1867,37 @@
       <c r="I30" s="1">
         <v>50000</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="J30" s="1">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
       <c r="K30" s="1">
         <v>2.04</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="1"/>
+        <f t="shared" si="2"/>
+        <v>0.96078431372549011</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="3"/>
+        <v>3.92</v>
+      </c>
+      <c r="O30">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M33" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M34" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>